<commit_message>
change in distance algorithm
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -3371,7 +3371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4541,6 +4541,106 @@
         <v>165</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>123_Car</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Minya</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>1234_Car</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Minya</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>123_Car</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Minya</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>123_Car</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Minya</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>123_Car</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Minya</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>